<commit_message>
updated national story with new data for 3 states
</commit_message>
<xml_diff>
--- a/data/Data for web team 2021 v5.xlsx
+++ b/data/Data for web team 2021 v5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csgorg.sharepoint.com/sites/Team-JC-Research/Shared Documents/50 State Revocations Project/50 State Survey (2021)/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1251" documentId="8_{719CCFE4-880F-4C83-BEAE-0D6CBEEAE7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F84454AD-D8EC-444B-97A8-4C5D6B0B46CA}"/>
+  <xr:revisionPtr revIDLastSave="1298" documentId="8_{719CCFE4-880F-4C83-BEAE-0D6CBEEAE7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FDE7080-FBB8-4410-8B32-9448A108628F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Admissions 2018" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="129">
   <si>
     <t>State Abbrev</t>
   </si>
@@ -448,7 +448,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -476,12 +476,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFED7D31"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -600,7 +594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -710,11 +704,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1877,8 +1866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IR52"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView showGridLines="0" topLeftCell="B26" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -2960,14 +2949,26 @@
       <c r="B36" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
+      <c r="C36" s="26">
+        <v>20697</v>
+      </c>
+      <c r="D36" s="26">
+        <v>6335</v>
+      </c>
+      <c r="E36" s="26">
+        <v>3234</v>
+      </c>
       <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
+      <c r="G36" s="26">
+        <v>3234</v>
+      </c>
+      <c r="H36" s="26">
+        <v>3101</v>
+      </c>
       <c r="I36" s="28"/>
-      <c r="J36" s="28"/>
+      <c r="J36" s="28">
+        <v>3101</v>
+      </c>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1">
       <c r="A37" s="23" t="s">
@@ -3432,8 +3433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:IS52"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView showGridLines="0" topLeftCell="B26" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -4525,14 +4526,26 @@
       <c r="B36" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
+      <c r="C36" s="26">
+        <v>20194</v>
+      </c>
+      <c r="D36" s="26">
+        <v>6357</v>
+      </c>
+      <c r="E36" s="26">
+        <v>3019</v>
+      </c>
       <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
+      <c r="G36" s="26">
+        <v>3019</v>
+      </c>
+      <c r="H36" s="26">
+        <v>3338</v>
+      </c>
       <c r="I36" s="26"/>
-      <c r="J36" s="26"/>
+      <c r="J36" s="26">
+        <v>3338</v>
+      </c>
       <c r="K36" s="26"/>
     </row>
     <row r="37" spans="1:11" ht="15" customHeight="1">
@@ -5009,8 +5022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IT53"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B33" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView showGridLines="0" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -6497,19 +6510,37 @@
       <c r="B36" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
+      <c r="C36" s="26">
+        <v>14022</v>
+      </c>
+      <c r="D36" s="26">
+        <v>4779</v>
+      </c>
+      <c r="E36" s="26">
+        <v>1931</v>
+      </c>
       <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
+      <c r="G36" s="26">
+        <v>1931</v>
+      </c>
+      <c r="H36" s="26">
+        <v>2848</v>
+      </c>
       <c r="I36" s="26"/>
-      <c r="J36" s="26"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="28"/>
-      <c r="M36" s="28"/>
+      <c r="J36" s="26">
+        <v>2848</v>
+      </c>
+      <c r="K36" s="32">
+        <v>2020</v>
+      </c>
+      <c r="L36" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="M36" s="28">
+        <v>12</v>
+      </c>
       <c r="N36" s="37" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="O36" s="28"/>
       <c r="P36" s="28"/>
@@ -7186,8 +7217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:IT55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+    <sheetView showGridLines="0" topLeftCell="B29" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -16698,14 +16729,26 @@
       <c r="B36" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
+      <c r="C36" s="5">
+        <v>48954</v>
+      </c>
+      <c r="D36" s="5">
+        <v>4342</v>
+      </c>
+      <c r="E36" s="5">
+        <v>2877</v>
+      </c>
       <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
+      <c r="G36" s="5">
+        <v>2877</v>
+      </c>
+      <c r="H36" s="5">
+        <v>1465</v>
+      </c>
       <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
+      <c r="J36" s="5">
+        <v>1465</v>
+      </c>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="20"/>
@@ -22078,8 +22121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:IT55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView showGridLines="0" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -31591,14 +31634,26 @@
       <c r="B36" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
+      <c r="C36" s="5">
+        <v>48697</v>
+      </c>
+      <c r="D36" s="5">
+        <v>4438</v>
+      </c>
+      <c r="E36" s="5">
+        <v>2870</v>
+      </c>
       <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
+      <c r="G36" s="5">
+        <v>2870</v>
+      </c>
+      <c r="H36" s="5">
+        <v>1568</v>
+      </c>
       <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
+      <c r="J36" s="5">
+        <v>1568</v>
+      </c>
       <c r="K36" s="4"/>
       <c r="L36" s="20"/>
       <c r="M36" s="20"/>
@@ -36955,8 +37010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:IT65"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="K51" sqref="K51"/>
+    <sheetView showGridLines="0" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -46476,16 +46531,28 @@
       <c r="B36" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="61"/>
-      <c r="D36" s="61"/>
-      <c r="E36" s="61"/>
+      <c r="C36" s="61">
+        <v>43665</v>
+      </c>
+      <c r="D36" s="61">
+        <v>3662</v>
+      </c>
+      <c r="E36" s="61">
+        <v>2146</v>
+      </c>
       <c r="F36" s="61"/>
-      <c r="G36" s="61"/>
-      <c r="H36" s="61"/>
+      <c r="G36" s="61">
+        <v>2146</v>
+      </c>
+      <c r="H36" s="61">
+        <v>1516</v>
+      </c>
       <c r="I36" s="61"/>
-      <c r="J36" s="61"/>
+      <c r="J36" s="61">
+        <v>1516</v>
+      </c>
       <c r="K36" s="59" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L36" s="59"/>
       <c r="N36" s="20"/>
@@ -54235,8 +54302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EBA7079-3894-49AA-98D1-2B5E43F1BAE6}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C36" sqref="A36:C36"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -54634,14 +54701,14 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="69" t="s">
+      <c r="A36" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="70" t="s">
-        <v>117</v>
-      </c>
-      <c r="C36" s="71" t="s">
-        <v>117</v>
+      <c r="B36" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="41" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -54823,21 +54890,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085A98439AFA81E498F77D25C786519F4" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2eee30f09807eeac4a01227db7fe7da3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="761c6e68-1cb6-4689-a9f8-1fc6e959a784" xmlns:ns3="92180e4e-06c3-4953-9d7f-e8282e53295e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="12701c335ef03a3ee46b176a305484f3" ns2:_="" ns3:_="">
     <xsd:import namespace="761c6e68-1cb6-4689-a9f8-1fc6e959a784"/>
@@ -55048,14 +55106,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF3EFDD-5B69-4990-915C-5FBC000951BA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28AF7866-3992-45B4-9764-3FF39FD33CFF}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28AF7866-3992-45B4-9764-3FF39FD33CFF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61908B07-54D0-41B3-8455-6EB578778097}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61908B07-54D0-41B3-8455-6EB578778097}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF3EFDD-5B69-4990-915C-5FBC000951BA}"/>
 </file>
</xml_diff>